<commit_message>
bonus - good reaction time
</commit_message>
<xml_diff>
--- a/results/mereni_jmena.xlsx
+++ b/results/mereni_jmena.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5. ročník\DP\Bitalino\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6D9D06-48FC-4BEC-9FF3-38B0C62AA794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09306FF0-2CD2-4E05-9636-52E32ED82F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1572" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
   <si>
     <t>Jméno</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Verča Kol.</t>
   </si>
   <si>
-    <t>Verča Poš.</t>
-  </si>
-  <si>
     <t>Eliška Kl.</t>
   </si>
   <si>
@@ -135,18 +132,12 @@
     <t>středa?</t>
   </si>
   <si>
-    <t>úterý 18:00</t>
-  </si>
-  <si>
     <t>Pozn.2</t>
   </si>
   <si>
     <t>Ondra</t>
   </si>
   <si>
-    <t xml:space="preserve">utery </t>
-  </si>
-  <si>
     <t xml:space="preserve">Já </t>
   </si>
   <si>
@@ -154,6 +145,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>*****</t>
   </si>
 </sst>
 </file>
@@ -233,16 +227,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8B49674-9B0A-431E-A891-02FA60295CAA}" name="Tabulka1" displayName="Tabulka1" ref="A1:H24" totalsRowShown="0">
-  <autoFilter ref="A1:H24" xr:uid="{4C9C056E-3CA8-4D18-AC38-73E4C2C3B30F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8B49674-9B0A-431E-A891-02FA60295CAA}" name="Tabulka1" displayName="Tabulka1" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23" xr:uid="{4C9C056E-3CA8-4D18-AC38-73E4C2C3B30F}">
     <filterColumn colId="7">
       <filters>
         <filter val="ANO"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H23">
-    <sortCondition descending="1" ref="A1:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+    <sortCondition descending="1" ref="A1:A23"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{283AF5DB-E9C5-43A9-BED7-74352F5AFB1F}" name="Jméno"/>
@@ -521,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +553,7 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,93 +578,93 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
         <v>25</v>
-      </c>
-      <c r="B3">
-        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="E5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>35</v>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -678,24 +672,24 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>25</v>
@@ -712,7 +706,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>25</v>
@@ -720,8 +714,8 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -729,41 +723,41 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -771,116 +765,117 @@
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E14" s="1"/>
       <c r="F14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
-        <v>39</v>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>16</v>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B19" s="2">
         <v>37</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" t="s">
+      <c r="G19" s="2"/>
+      <c r="H19" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -889,36 +884,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="H23" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>